<commit_message>
Atualização da Ata de Reuniões
</commit_message>
<xml_diff>
--- a/Documentação/Atas/Atas de Reuniões - Sprint (Atualizada).xlsx
+++ b/Documentação/Atas/Atas de Reuniões - Sprint (Atualizada).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pehso\Downloads\git09\MushRoomCompany\Documentação\Atas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pehso\Downloads\git backaup\MushRoomCompany\Documentação\Atas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2B74A3-3A06-4352-A868-525B53FBBAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB7707E-851F-4085-9798-5BB04C1D1516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D442432-517F-4F4B-B9FC-9178A77BD6D6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Alteramos o PO Daniel e o Scrum Master Pedro ;  Adicionamos novos requisitos no Project Backlog; foram delegadas as funçoes da semana para cada membro;</t>
   </si>
@@ -147,6 +147,21 @@
   </si>
   <si>
     <t>SPRINT-B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foi reforçados com os  membros ausentes na ultima reunião os conteudos que serão desenvolvidos na semana e o que cada membro vai desenvolver; </t>
+  </si>
+  <si>
+    <t>Validamos e reforçamos os prazos de entrega da semana ;</t>
+  </si>
+  <si>
+    <t>08/10 (Segunda-Feira)</t>
+  </si>
+  <si>
+    <t>09/10 (Terça-Feira)</t>
+  </si>
+  <si>
+    <t>10/10 (Quarta-Feira)</t>
   </si>
 </sst>
 </file>
@@ -306,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -337,8 +352,11 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -347,6 +365,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -665,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C5EB23-2437-4857-BB14-413C2F1BA111}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -681,42 +702,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1">
       <c r="A5" s="11" t="s">
@@ -760,7 +781,7 @@
       </c>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="112.5">
+    <row r="7" spans="1:7" ht="126.75" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -779,7 +800,7 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="112.5">
+    <row r="8" spans="1:7" ht="144.75" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
@@ -798,7 +819,7 @@
       </c>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" ht="79.5" customHeight="1">
+    <row r="9" spans="1:7" ht="108.75" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
@@ -831,19 +852,19 @@
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" ht="45" customHeight="1">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="15"/>
-    </row>
-    <row r="12" spans="1:7" ht="112.5" customHeight="1">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="1:7" ht="144.75" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B12" s="4">
         <v>0.69444444444444453</v>
@@ -864,19 +885,33 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="60.75" customHeight="1">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+    <row r="13" spans="1:7" ht="138" customHeight="1">
+      <c r="A13" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.71180555555555547</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" ht="60" customHeight="1">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="F13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="112.5" customHeight="1">
+      <c r="A14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>

</xml_diff>

<commit_message>
Atualização Diária da Ata de reuniões
</commit_message>
<xml_diff>
--- a/Documentação/Atas/Atas de Reuniões - Sprint (Atualizada).xlsx
+++ b/Documentação/Atas/Atas de Reuniões - Sprint (Atualizada).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pehso\Downloads\git backaup\MushRoomCompany\Documentação\Atas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB7707E-851F-4085-9798-5BB04C1D1516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD90245-BA08-45A6-848A-89A506FF9BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D442432-517F-4F4B-B9FC-9178A77BD6D6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Alteramos o PO Daniel e o Scrum Master Pedro ;  Adicionamos novos requisitos no Project Backlog; foram delegadas as funçoes da semana para cada membro;</t>
   </si>
@@ -162,6 +162,22 @@
   </si>
   <si>
     <t>10/10 (Quarta-Feira)</t>
+  </si>
+  <si>
+    <t>Davi</t>
+  </si>
+  <si>
+    <t>Arthur
+Daniel
+Leonardo
+Matteus
+Pedro</t>
+  </si>
+  <si>
+    <t>Definimos como sera desenvolvido a modelagem logíca e script do banco de dados (Métricas dos sensores ) e quem desenvolvera;</t>
+  </si>
+  <si>
+    <t>Compartilhamos experiencia sobre o desenvolvimento do projeto;  definimos como será feito o banco de dados (Métricas dos sensores) ;</t>
   </si>
 </sst>
 </file>
@@ -686,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C5EB23-2437-4857-BB14-413C2F1BA111}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -906,16 +922,28 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="112.5" customHeight="1">
+    <row r="14" spans="1:7" ht="142.5" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="B14" s="4">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.4375</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Alterando a Ata da Sprint B, detalhando o que foi discutido
</commit_message>
<xml_diff>
--- a/Documentação/Atas/Atas de Reuniões - Sprint (Atualizada).xlsx
+++ b/Documentação/Atas/Atas de Reuniões - Sprint (Atualizada).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pehso\Downloads\git backaup\MushRoomCompany\Documentação\Atas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viibe\Desktop\GitHub\MushRoomCompany\Documentação\Atas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD90245-BA08-45A6-848A-89A506FF9BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49AC09B-743D-4BBC-A785-EC6953FFFD5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D442432-517F-4F4B-B9FC-9178A77BD6D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4D442432-517F-4F4B-B9FC-9178A77BD6D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Atas de reuniões" sheetId="1" r:id="rId1"/>
@@ -20,26 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
-  <si>
-    <t>Alteramos o PO Daniel e o Scrum Master Pedro ;  Adicionamos novos requisitos no Project Backlog; foram delegadas as funçoes da semana para cada membro;</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Leonardo</t>
   </si>
@@ -57,29 +43,7 @@
     <t>06/10 (Sexta-Feira)</t>
   </si>
   <si>
-    <t>Comentamos sobre o que cada um já havia feito; Decidimos que a Dashboard teria um Dropdown</t>
-  </si>
-  <si>
     <t>05/10 (Quinta-Feira)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Alinhamento de opinião;
-Atualização na documentação;
- O Git foi atualizado;
- O Trello foi reorganizado;</t>
-    </r>
   </si>
   <si>
     <t>Arthur
@@ -93,32 +57,9 @@
     <t>04/10 (Quarta-Feira)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve"> 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Docs-Merriweather"/>
-      </rPr>
-      <t xml:space="preserve"> Discutimos sobre as nossas tarefas;
- Discutimos sobre a organização do Trello;
- Falamos sobre a documentação;</t>
-    </r>
-  </si>
-  <si>
     <t>03/10 (Terça-Feira)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Alteramos o PO Arthur e o Scrum Master Leonardo;
- Alteramos a importância do requisito da Dashboard;
- Discutimos sobre a documentação, em especifíco o Backlog;
-Atualizamos o Backlog;
-</t>
-  </si>
-  <si>
     <t>Assuntos Decididos</t>
   </si>
   <si>
@@ -141,18 +82,6 @@
   </si>
   <si>
     <t>ATAS DE REUNIÕES - PROJETO MUSHROOM</t>
-  </si>
-  <si>
-    <t>Dividimos o armazenamento do banco de dados e a conexão do banco de dados em 2 requisitos um para armazenar dados dos sensore e outro para os dados dos clientes;  Subdividomos o site em dois requisitos (Header e footer);</t>
-  </si>
-  <si>
-    <t>SPRINT-B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">foi reforçados com os  membros ausentes na ultima reunião os conteudos que serão desenvolvidos na semana e o que cada membro vai desenvolver; </t>
-  </si>
-  <si>
-    <t>Validamos e reforçamos os prazos de entrega da semana ;</t>
   </si>
   <si>
     <t>08/10 (Segunda-Feira)</t>
@@ -174,17 +103,74 @@
 Pedro</t>
   </si>
   <si>
-    <t>Definimos como sera desenvolvido a modelagem logíca e script do banco de dados (Métricas dos sensores ) e quem desenvolvera;</t>
-  </si>
-  <si>
-    <t>Compartilhamos experiencia sobre o desenvolvimento do projeto;  definimos como será feito o banco de dados (Métricas dos sensores) ;</t>
+    <t>SPRINT- C</t>
+  </si>
+  <si>
+    <t>SPRINT- B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validamos e reforçamos os prazos de entrega da semana </t>
+  </si>
+  <si>
+    <t>Definimos como sera desenvolvido a modelagem logíca e script do banco de dados (Métricas dos sensores ) e quem desenvolvera</t>
+  </si>
+  <si>
+    <t>Alteramos o PO Daniel e o Scrum Master Pedro ;                        Adicionamos novos requisitos no Project Backlog;                                             Foram delegadas as funçoes da semana para cada membro.</t>
+  </si>
+  <si>
+    <t>Comentamos sobre o que cada um já havia feito;                             Decidimos que a Dashboard teria um menu Dropdown.</t>
+  </si>
+  <si>
+    <t>Alinhamento de opinião;
+Atualização na documentação;
+ O Git foi atualizado;
+ O Trello foi reorganizado.</t>
+  </si>
+  <si>
+    <t>Discutimos sobre as nossas tarefas;
+ Discutimos sobre a organização do Trello;
+ Falamos sobre a documentação.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alteramos o PO Arthur e o Scrum Master Leonardo;
+ Alteramos a importância do requisito da Dashboard;
+ Discutimos sobre a documentação, em especifíco o Backlog;
+Atualizamos o Backlog.
+</t>
+  </si>
+  <si>
+    <t>foi reforçados com os  membros ausentes na ultima reunião os conteudos que serão desenvolvidos na semana e o que cada membro vai desenvolver.</t>
+  </si>
+  <si>
+    <t>Compartilhamos experiência sobre o desenvolvimento do projeto;  Definimos como será feito o banco de dados (Métricas dos sensores) .</t>
+  </si>
+  <si>
+    <t>Dividimos o armazenamento do banco de dados e a conexão do banco de dados em 2 requisitos um para armazenar dados dos sensore e outro para os dados dos clientes;                                                                                                       Subdivídimos o site em dois requisitos (Header e footer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falamos sobre as atividades finalizadas e as atrasadas;                                        </t>
+  </si>
+  <si>
+    <t>Falamos sobre o que cada um de nós havia realizado.</t>
+  </si>
+  <si>
+    <t>Partilhamos dos nossos feitos novamente e entramos em um acordo que a nossa Dashboard teria um menu Dropdown pois separariamos os setores para que fique mais intuitivo para o cliente.</t>
+  </si>
+  <si>
+    <t>Conversamos sobre as nossas ideias a respeito do projeto e tentamos alinhar nossas ideias para que fique agradável para todos, atualizamos a documentação com a alteração dos nomes dos integrantes do grupo, o Git foi atualizado e orientado que todos atualizasem sempre que possível, o Trello foi Reorganizado como haviamos falando na Daily anterior.</t>
+  </si>
+  <si>
+    <t>Partilhamos dos nossos feitos a respeito das tarefas propostas pelo Scrum, O quê já haviamos feito, se estavamos com dificuldades ou precisariamos de ajuda pra executa-lás, falamos também sobre a organização do Trello e como ficariam e por fim falamos sobre a documentação onde seria feito algumas alterações.</t>
+  </si>
+  <si>
+    <t>Decidimos que haveria alteração do Scrum e do PO, após isso discutimos sobre os requisitos e achamos que era melhor trocar a importância da Dashboad pois entramos em um acordo que seria Importante, também, foi decidido alterar algumas coisas do Backlog.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,24 +193,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Docs-Merriweather"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Docs-Merriweather"/>
-    </font>
-    <font>
       <b/>
       <sz val="48"/>
       <color theme="1"/>
@@ -242,6 +210,21 @@
     <font>
       <sz val="36"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -337,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -352,13 +335,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -374,17 +350,29 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -700,13 +688,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C5EB23-2437-4857-BB14-413C2F1BA111}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" customWidth="1"/>
@@ -717,125 +705,121 @@
     <col min="7" max="7" width="87.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-    </row>
-    <row r="5" spans="1:7" ht="30" customHeight="1">
-      <c r="A5" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="11" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+    </row>
+    <row r="5" spans="1:7" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
+    </row>
+    <row r="6" spans="1:7" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" s="9" customFormat="1" ht="172.5" customHeight="1">
-      <c r="A6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="4">
-        <v>0.69444444444444453</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="1:7" ht="126.75" customHeight="1">
+    </row>
+    <row r="7" spans="1:7" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B7" s="4">
         <v>0.69444444444444453</v>
       </c>
       <c r="C7" s="4">
-        <v>0.70486111111111116</v>
+        <v>0.75</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" ht="144.75" customHeight="1">
+        <v>5</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
         <v>0.69444444444444453</v>
       </c>
       <c r="C8" s="4">
-        <v>0.70624999999999993</v>
+        <v>0.70486111111111116</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" ht="108.75" customHeight="1">
+      <c r="F8" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
@@ -843,16 +827,20 @@
         <v>0.69444444444444453</v>
       </c>
       <c r="C9" s="4">
-        <v>0.70347222222222217</v>
-      </c>
-      <c r="D9" s="1"/>
+        <v>0.70624999999999993</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" ht="89.25" customHeight="1">
+        <v>27</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
@@ -860,95 +848,123 @@
         <v>0.69444444444444453</v>
       </c>
       <c r="C10" s="4">
+        <v>0.70347222222222217</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="C11" s="4">
         <v>0.7055555555555556</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" ht="45" customHeight="1">
-      <c r="A11" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="16"/>
-    </row>
-    <row r="12" spans="1:7" ht="144.75" customHeight="1">
-      <c r="A12" s="5" t="s">
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:7" ht="138" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="4">
-        <v>0.69444444444444453</v>
-      </c>
-      <c r="C12" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="138" customHeight="1">
-      <c r="A13" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="4">
+      <c r="G13" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="4">
         <v>0.70138888888888884</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C14" s="4">
         <v>0.71180555555555547</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="13" t="s">
+      <c r="D14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="3" t="s">
+    </row>
+    <row r="15" spans="1:7" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.4375</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="142.5" customHeight="1">
-      <c r="A14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="4">
-        <v>0.43055555555555558</v>
-      </c>
-      <c r="C14" s="4">
-        <v>0.4375</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A11:G11"/>
+  <mergeCells count="3">
+    <mergeCell ref="A12:G12"/>
     <mergeCell ref="A1:G4"/>
+    <mergeCell ref="A5:G5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização do plano de acao
</commit_message>
<xml_diff>
--- a/Documentação/Atas/Atas de Reuniões - Sprint (Atualizada).xlsx
+++ b/Documentação/Atas/Atas de Reuniões - Sprint (Atualizada).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viibe\Desktop\GitHub\MushRoomCompany\Documentação\Atas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{322D864C-E947-47D6-8583-93106120E14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B6258E4-FCE4-4805-8A1E-B0275D3B8ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4D442432-517F-4F4B-B9FC-9178A77BD6D6}"/>
   </bookViews>
@@ -36,12 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
   <si>
     <t>ATAS DE REUNIÕES - PROJETO MUSHROOM</t>
   </si>
   <si>
-    <t>SPRINT- B</t>
+    <t>SPRINT- A</t>
   </si>
   <si>
     <t xml:space="preserve">Dia </t>
@@ -76,6 +76,28 @@
 Pedro</t>
   </si>
   <si>
+    <t>Foi discutido a rotação das funções PO e Scrum Master entre os membros da equipe
+Foi discutido o problema de comunicação da equipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foram decididos o Scrum Master e o Product owner.
+P.O (Arthur Gabriel), Scrum Master (Leonardo Rodrigues)
+Definindo a Ata de Reunião </t>
+  </si>
+  <si>
+    <t>03/10 (Terça-Feira)</t>
+  </si>
+  <si>
+    <t>Foi discutido como estava sendo feito as tarefas de cada integrante e se todos estavam conseguindo fazer o que foi designado na semana</t>
+  </si>
+  <si>
+    <t>Partilhamos dos nossos feitos a respeito das tarefas propostas pelo Scrum, O quê já haviamos feito, se estavamos com dificuldades ou precisariamos de ajuda pra executa-lás. 
+Concordamos que precisariamos revisar novamente os backlog de requisitos</t>
+  </si>
+  <si>
+    <t>SPRINT- B</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alteramos o PO Arthur e o Scrum Master Leonardo;
  Alteramos a importância do requisito da Dashboard;
  Discutimos sobre a documentação, em especifíco o Backlog;
@@ -86,9 +108,6 @@
     <t>Decidimos que haveria alteração do Scrum e do PO, após isso discutimos sobre os requisitos e achamos que era melhor trocar a importância da Dashboad pois entramos em um acordo que seria Importante, também, foi decidido alterar algumas coisas do Backlog.</t>
   </si>
   <si>
-    <t>03/10 (Terça-Feira)</t>
-  </si>
-  <si>
     <t>Discutimos sobre as nossas tarefas;
  Discutimos sobre a organização do Trello;
  Falamos sobre a documentação.</t>
@@ -224,7 +243,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,14 +298,6 @@
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -382,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -417,6 +428,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -424,12 +438,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -748,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C5EB23-2437-4857-BB14-413C2F1BA111}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A15" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -844,7 +852,7 @@
         <v>0.69444444444444453</v>
       </c>
       <c r="C7" s="10">
-        <v>0.75</v>
+        <v>0.8125</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>10</v>
@@ -865,7 +873,7 @@
         <v>0.69444444444444453</v>
       </c>
       <c r="C8" s="10">
-        <v>0.70486111111111116</v>
+        <v>0.70138888888888884</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>10</v>
@@ -879,202 +887,202 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="123" customHeight="1">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="10">
-        <v>0.69444444444444453</v>
-      </c>
-      <c r="C9" s="10">
-        <v>0.70624999999999993</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" ht="124.5" customHeight="1">
-      <c r="A10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="10">
-        <v>0.69444444444444453</v>
-      </c>
-      <c r="C10" s="10">
-        <v>0.70347222222222217</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>21</v>
+      <c r="A10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="144.75" customHeight="1">
       <c r="A11" s="9" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B11" s="10">
         <v>0.69444444444444453</v>
       </c>
       <c r="C11" s="10">
-        <v>0.7055555555555556</v>
+        <v>0.75</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="96.75" customHeight="1">
-      <c r="A12" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
+      <c r="A12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="10">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="138" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B13" s="10">
         <v>0.69444444444444453</v>
       </c>
       <c r="C13" s="10">
-        <v>0.75</v>
+        <v>0.70624999999999993</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E13" s="11"/>
       <c r="F13" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="150" customHeight="1">
-      <c r="A14" s="15" t="s">
-        <v>31</v>
+      <c r="A14" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="B14" s="10">
-        <v>0.70138888888888884</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="C14" s="10">
-        <v>0.71180555555555547</v>
+        <v>0.70347222222222217</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="108.75" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B15" s="10">
-        <v>0.43055555555555558</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="C15" s="10">
-        <v>0.4375</v>
+        <v>0.7055555555555556</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E15" s="11"/>
       <c r="F15" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="46.5">
-      <c r="A16" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="14"/>
+      <c r="A16" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="15"/>
     </row>
     <row r="17" spans="1:7" ht="94.5">
       <c r="A17" s="9" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B17" s="10">
         <v>0.69444444444444453</v>
       </c>
       <c r="C17" s="10">
-        <v>0.74305555555555547</v>
+        <v>0.75</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="F17" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="113.25">
-      <c r="A18" s="15" t="s">
-        <v>43</v>
+      <c r="A18" s="12" t="s">
+        <v>36</v>
       </c>
       <c r="B18" s="10">
-        <v>0.43055555555555558</v>
+        <v>0.70138888888888884</v>
       </c>
       <c r="C18" s="10">
-        <v>0.4375</v>
+        <v>0.71180555555555547</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="11"/>
       <c r="F18" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="94.5">
       <c r="A19" s="9" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B19" s="10">
         <v>0.43055555555555558</v>
@@ -1083,46 +1091,118 @@
         <v>0.4375</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="F19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="46.5">
+      <c r="A20" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="15"/>
+    </row>
+    <row r="21" spans="1:7" ht="94.5">
+      <c r="A21" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="10">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="C21" s="10">
+        <v>0.74305555555555547</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G19" s="1" t="s">
+    </row>
+    <row r="22" spans="1:7" ht="113.25">
+      <c r="A22" s="12" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="94.5">
-      <c r="A20" s="9" t="s">
+      <c r="B22" s="10">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="C22" s="10">
+        <v>0.4375</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="10">
+      <c r="G22" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="94.5">
+      <c r="A23" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="10">
         <v>0.43055555555555558</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C23" s="10">
         <v>0.4375</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="C24" s="16"/>
+      <c r="D23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="94.5">
+      <c r="A24" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="10">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="C24" s="10">
+        <v>0.4375</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A12:G12"/>
+  <mergeCells count="3">
     <mergeCell ref="A1:G4"/>
+    <mergeCell ref="A9:G9"/>
     <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A16:G16"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update dashboard e documentação
</commit_message>
<xml_diff>
--- a/Documentação/Atas/Atas de Reuniões - Sprint (Atualizada).xlsx
+++ b/Documentação/Atas/Atas de Reuniões - Sprint (Atualizada).xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27016"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viibe\Desktop\GitHub\MushRoomCompany\Documentação\Atas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\Desktop\Material Sptech\Projetos\MushRoomCompany\Documentação\Atas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B6258E4-FCE4-4805-8A1E-B0275D3B8ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4D442432-517F-4F4B-B9FC-9178A77BD6D6}"/>
+    <workbookView minimized="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="Atas de reuniões" sheetId="1" r:id="rId1"/>
@@ -242,8 +241,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,12 +400,36 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -414,30 +437,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -753,111 +752,111 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C5EB23-2437-4857-BB14-413C2F1BA111}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="34.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="87.28515625" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="36.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="87.28515625" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="96.75" customHeight="1">
-      <c r="A5" s="5" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="1:7" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" ht="30" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
+    </row>
+    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="126.75" customHeight="1">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:7" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="6">
         <v>0.69444444444444453</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="6">
         <v>0.8125</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="11"/>
+      <c r="E7" s="7"/>
       <c r="F7" s="1" t="s">
         <v>11</v>
       </c>
@@ -865,20 +864,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="144.75" customHeight="1">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:7" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="6">
         <v>0.69444444444444453</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="6">
         <v>0.70138888888888884</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="11"/>
+      <c r="E8" s="7"/>
       <c r="F8" s="2" t="s">
         <v>14</v>
       </c>
@@ -886,54 +885,54 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="123" customHeight="1">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:7" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" ht="124.5" customHeight="1">
-      <c r="A10" s="8" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+    </row>
+    <row r="10" spans="1:7" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="144.75" customHeight="1">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:7" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="6">
         <v>0.69444444444444453</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="6">
         <v>0.75</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="11"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="1" t="s">
         <v>17</v>
       </c>
@@ -941,20 +940,20 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="96.75" customHeight="1">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:7" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="6">
         <v>0.69444444444444453</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="6">
         <v>0.70486111111111116</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="11"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="2" t="s">
         <v>19</v>
       </c>
@@ -962,20 +961,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="138" customHeight="1">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:7" ht="138" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="6">
         <v>0.69444444444444453</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="6">
         <v>0.70624999999999993</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="11"/>
+      <c r="E13" s="7"/>
       <c r="F13" s="1" t="s">
         <v>22</v>
       </c>
@@ -983,20 +982,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="150" customHeight="1">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:7" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="6">
         <v>0.69444444444444453</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="6">
         <v>0.70347222222222217</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="11"/>
+      <c r="E14" s="7"/>
       <c r="F14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1004,20 +1003,20 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="108.75" customHeight="1">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:7" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="6">
         <v>0.69444444444444453</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="6">
         <v>0.7055555555555556</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="11"/>
+      <c r="E15" s="7"/>
       <c r="F15" s="1" t="s">
         <v>28</v>
       </c>
@@ -1025,25 +1024,25 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="46.5">
-      <c r="A16" s="13" t="s">
+    <row r="16" spans="1:7" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="15"/>
-    </row>
-    <row r="17" spans="1:7" ht="94.5">
-      <c r="A17" s="9" t="s">
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="1:7" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="6">
         <v>0.69444444444444453</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="6">
         <v>0.75</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1059,20 +1058,20 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="113.25">
-      <c r="A18" s="12" t="s">
+    <row r="18" spans="1:7" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="6">
         <v>0.70138888888888884</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="6">
         <v>0.71180555555555547</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="11"/>
+      <c r="E18" s="7"/>
       <c r="F18" s="1" t="s">
         <v>37</v>
       </c>
@@ -1080,14 +1079,14 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="94.5">
-      <c r="A19" s="9" t="s">
+    <row r="19" spans="1:7" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="6">
         <v>0.43055555555555558</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="6">
         <v>0.4375</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1103,25 +1102,25 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="46.5">
-      <c r="A20" s="13" t="s">
+    <row r="20" spans="1:7" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="15"/>
-    </row>
-    <row r="21" spans="1:7" ht="94.5">
-      <c r="A21" s="9" t="s">
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="1:7" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="6">
         <v>0.69444444444444453</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="6">
         <v>0.74305555555555547</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1135,20 +1134,20 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="113.25">
-      <c r="A22" s="12" t="s">
+    <row r="22" spans="1:7" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="6">
         <v>0.43055555555555558</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="6">
         <v>0.4375</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="11"/>
+      <c r="E22" s="7"/>
       <c r="F22" s="1" t="s">
         <v>49</v>
       </c>
@@ -1156,14 +1155,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="94.5">
-      <c r="A23" s="9" t="s">
+    <row r="23" spans="1:7" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="6">
         <v>0.43055555555555558</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="6">
         <v>0.4375</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1177,14 +1176,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="94.5">
-      <c r="A24" s="9" t="s">
+    <row r="24" spans="1:7" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="6">
         <v>0.43055555555555558</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="6">
         <v>0.4375</v>
       </c>
       <c r="D24" s="1" t="s">

</xml_diff>

<commit_message>
Banco de Dados Terminado
</commit_message>
<xml_diff>
--- a/Documentação/Atas/Atas de Reuniões - Sprint (Atualizada).xlsx
+++ b/Documentação/Atas/Atas de Reuniões - Sprint (Atualizada).xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPRINT2\MushRoomCompany\Documentação\Atas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\Desktop\Material Sptech\Projetos\MushRoomCompany\Documentação\Atas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524AAB95-66D8-4097-A96A-78B8BA51C071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Atas de reuniões" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
   <si>
     <t>ATAS DE REUNIÕES - PROJETO MUSHROOM</t>
   </si>
@@ -252,7 +251,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -769,11 +768,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="C24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,7 +1233,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>45223</v>
       </c>
@@ -1243,6 +1242,9 @@
       </c>
       <c r="C26" s="13">
         <v>0.72916666666666663</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>62</v>

</xml_diff>